<commit_message>
Assignment4: A assignment started
</commit_message>
<xml_diff>
--- a/Assignment4B/TestSummary.xlsx
+++ b/Assignment4B/TestSummary.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\csharp3-mau\Assignment4B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBB9A28-64F3-469F-BBEE-3E7290AB7ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201E2E83-9EB1-4ACC-97C1-9A3AB0ED8A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="13695" windowWidth="17520" windowHeight="14265" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AlbumManager" sheetId="1" r:id="rId1"/>
     <sheet name="AlbumService" sheetId="2" r:id="rId2"/>
+    <sheet name="A-Grade" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Method Name</t>
   </si>
@@ -51,24 +52,6 @@
     <t>Action</t>
   </si>
   <si>
-    <t>DeleteItem</t>
-  </si>
-  <si>
-    <t>Removes File at position</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>While writing test for AlbumManager I realized that SlideShowManager had the exact same implementation so decided to refactor so BaseManager implements the method</t>
-  </si>
-  <si>
-    <t>MoveItem</t>
-  </si>
-  <si>
-    <t>Moves a File to a new position in the colleciton</t>
-  </si>
-  <si>
     <t>Save</t>
   </si>
   <si>
@@ -91,6 +74,27 @@
   </si>
   <si>
     <t>Add check if Album.Files is null to prevent validation from failing</t>
+  </si>
+  <si>
+    <t>BugViewModel.Validate</t>
+  </si>
+  <si>
+    <t>I wanted to test my Validate logic</t>
+  </si>
+  <si>
+    <t>The result was to yet again make my private methods internal to be able to tests them. I also realized that both Save and Validate used a class property instead of an in-parameter, which would be more easily tested.</t>
+  </si>
+  <si>
+    <t>BugViewModel.Save</t>
+  </si>
+  <si>
+    <t>I wanted to test that Validate logic was ok and that the delegate was called</t>
+  </si>
+  <si>
+    <t>It failed because when calling OnSave, there were no delegate registered</t>
+  </si>
+  <si>
+    <t>Add check that OnSave is not null before invoking the event and also mock the event to prevent it from executing</t>
   </si>
 </sst>
 </file>
@@ -106,16 +110,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,18 +149,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dålig" xfId="1" builtinId="27"/>
@@ -438,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,46 +467,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -518,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B0A2D3A-B432-44C5-85D6-B6E9BA23BF4F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,16 +519,78 @@
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFB4D2D-2E05-46F9-A3E7-0FAD3A824927}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assignment 4: Ready for hand-in
</commit_message>
<xml_diff>
--- a/Assignment4B/TestSummary.xlsx
+++ b/Assignment4B/TestSummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\csharp3-mau\Assignment4B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201E2E83-9EB1-4ACC-97C1-9A3AB0ED8A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93D674F-7EC8-40C8-8D60-0EA73AB4F12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>Method Name</t>
   </si>
@@ -95,13 +95,40 @@
   </si>
   <si>
     <t>Add check that OnSave is not null before invoking the event and also mock the event to prevent it from executing</t>
+  </si>
+  <si>
+    <t>BugViewModel.ShowClosedReason</t>
+  </si>
+  <si>
+    <t>If status changed to Finished or Rejected then ShowCloseReason should be set to true</t>
+  </si>
+  <si>
+    <t>It was as expected</t>
+  </si>
+  <si>
+    <t>BugViewModel.Bug.CloseReason</t>
+  </si>
+  <si>
+    <t>If status changed from Finished or Rejected then Bug.CloseReason is set to empty string</t>
+  </si>
+  <si>
+    <t>MainViewModel.Bugs.CollectionChanged</t>
+  </si>
+  <si>
+    <t>When colletion change on Add/Delete the text indiciating how many bugs there are in the system should change</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>I made validate and save public methods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,25 +144,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,20 +162,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Dålig" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -539,10 +551,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFB4D2D-2E05-46F9-A3E7-0FAD3A824927}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +589,9 @@
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -591,6 +605,48 @@
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>